<commit_message>
update package 9 wrong address
</commit_message>
<xml_diff>
--- a/packages.xlsx
+++ b/packages.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miguel.dehoyos\Downloads\C950\New Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7D6FC3F-E74F-4587-BEDF-A00C8FAE7100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -184,13 +184,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -251,59 +257,152 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -316,7 +415,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -344,25 +443,17 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1412008" y="60961"/>
-          <a:ext cx="3792452" cy="419968"/>
+          <a:off x="1362075" y="57150"/>
+          <a:ext cx="3533775" cy="419100"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+        <a:prstGeom prst="rect"/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -632,24 +723,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:H6"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.884285714285713" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="3.77734375" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.142857142857142" customWidth="1"/>
+    <col min="4" max="4" width="3.7142857142857144" customWidth="1"/>
+    <col min="5" max="5" width="5.142857142857143" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" customWidth="1"/>
-    <col min="8" max="8" width="39.77734375" customWidth="1"/>
+    <col min="7" max="7" width="6.714285714285714" customWidth="1"/>
+    <col min="8" max="8" width="39.714285714285715" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:13" ht="14.4" customHeight="1">
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
@@ -661,7 +752,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:13" ht="14.4" customHeight="1">
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
@@ -673,7 +764,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:13" ht="14.4" customHeight="1">
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -685,7 +776,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15" customHeight="1">
       <c r="A4" s="14" t="s">
         <v>0</v>
       </c>
@@ -698,7 +789,7 @@
       <c r="H4" s="13"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="14.4" customHeight="1">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -709,7 +800,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15.6" customHeight="1">
       <c r="A6" s="12" t="s">
         <v>48</v>
       </c>
@@ -721,7 +812,7 @@
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="3" customFormat="1" ht="28.8" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>45</v>
       </c>
@@ -747,7 +838,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="12.9" customHeight="1">
       <c r="A9" s="9">
         <v>1</v>
       </c>
@@ -771,7 +862,7 @@
       </c>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="12.9" customHeight="1">
       <c r="A10" s="9">
         <v>2</v>
       </c>
@@ -795,7 +886,7 @@
       </c>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="12.9" customHeight="1">
       <c r="A11" s="9">
         <v>3</v>
       </c>
@@ -821,7 +912,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="12.9" customHeight="1">
       <c r="A12" s="9">
         <v>4</v>
       </c>
@@ -845,7 +936,7 @@
       </c>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="12.9" customHeight="1">
       <c r="A13" s="9">
         <v>5</v>
       </c>
@@ -869,7 +960,7 @@
       </c>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="12.9" customHeight="1">
       <c r="A14" s="9">
         <v>6</v>
       </c>
@@ -895,7 +986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="12.9" customHeight="1">
       <c r="A15" s="9">
         <v>7</v>
       </c>
@@ -919,7 +1010,7 @@
       </c>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="12.9" customHeight="1">
       <c r="A16" s="9">
         <v>8</v>
       </c>
@@ -943,7 +1034,7 @@
       </c>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="12.9" customHeight="1">
       <c r="A17" s="9">
         <v>9</v>
       </c>
@@ -969,7 +1060,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="12.9" customHeight="1">
       <c r="A18" s="9">
         <v>10</v>
       </c>
@@ -993,7 +1084,7 @@
       </c>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="12.9" customHeight="1">
       <c r="A19" s="9">
         <v>11</v>
       </c>
@@ -1017,7 +1108,7 @@
       </c>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="12.9" customHeight="1">
       <c r="A20" s="9">
         <v>12</v>
       </c>
@@ -1041,7 +1132,7 @@
       </c>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="12.9" customHeight="1">
       <c r="A21" s="9">
         <v>13</v>
       </c>
@@ -1065,7 +1156,7 @@
       </c>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="12.9" customHeight="1">
       <c r="A22" s="9">
         <v>14</v>
       </c>
@@ -1091,7 +1182,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="12.9" customHeight="1">
       <c r="A23" s="9">
         <v>15</v>
       </c>
@@ -1115,7 +1206,7 @@
       </c>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="12.9" customHeight="1">
       <c r="A24" s="9">
         <v>16</v>
       </c>
@@ -1141,7 +1232,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="12.9" customHeight="1">
       <c r="A25" s="9">
         <v>17</v>
       </c>
@@ -1165,7 +1256,7 @@
       </c>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="12.9" customHeight="1">
       <c r="A26" s="9">
         <v>18</v>
       </c>
@@ -1191,7 +1282,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="12.9" customHeight="1">
       <c r="A27" s="9">
         <v>19</v>
       </c>
@@ -1215,7 +1306,7 @@
       </c>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="12.9" customHeight="1">
       <c r="A28" s="9">
         <v>20</v>
       </c>
@@ -1241,7 +1332,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="12.9" customHeight="1">
       <c r="A29" s="9">
         <v>21</v>
       </c>
@@ -1265,7 +1356,7 @@
       </c>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="12.9" customHeight="1">
       <c r="A30" s="9">
         <v>22</v>
       </c>
@@ -1289,7 +1380,7 @@
       </c>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="12.9" customHeight="1">
       <c r="A31" s="9">
         <v>23</v>
       </c>
@@ -1313,7 +1404,7 @@
       </c>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="12.9" customHeight="1">
       <c r="A32" s="9">
         <v>24</v>
       </c>
@@ -1337,7 +1428,7 @@
       </c>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="12.9" customHeight="1">
       <c r="A33" s="9">
         <v>25</v>
       </c>
@@ -1363,7 +1454,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="12.9" customHeight="1">
       <c r="A34" s="9">
         <v>26</v>
       </c>
@@ -1387,7 +1478,7 @@
       </c>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="12.9" customHeight="1">
       <c r="A35" s="9">
         <v>27</v>
       </c>
@@ -1411,7 +1502,7 @@
       </c>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="12.9" customHeight="1">
       <c r="A36" s="9">
         <v>28</v>
       </c>
@@ -1437,7 +1528,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="12.9" customHeight="1">
       <c r="A37" s="9">
         <v>29</v>
       </c>
@@ -1461,7 +1552,7 @@
       </c>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="12.9" customHeight="1">
       <c r="A38" s="9">
         <v>30</v>
       </c>
@@ -1485,7 +1576,7 @@
       </c>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="12.9" customHeight="1">
       <c r="A39" s="9">
         <v>31</v>
       </c>
@@ -1509,7 +1600,7 @@
       </c>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="12.9" customHeight="1">
       <c r="A40" s="9">
         <v>32</v>
       </c>
@@ -1535,7 +1626,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="12.9" customHeight="1">
       <c r="A41" s="9">
         <v>33</v>
       </c>
@@ -1559,7 +1650,7 @@
       </c>
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="12.9" customHeight="1">
       <c r="A42" s="9">
         <v>34</v>
       </c>
@@ -1583,7 +1674,7 @@
       </c>
       <c r="H42" s="4"/>
     </row>
-    <row r="43" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="12.9" customHeight="1">
       <c r="A43" s="9">
         <v>35</v>
       </c>
@@ -1607,7 +1698,7 @@
       </c>
       <c r="H43" s="4"/>
     </row>
-    <row r="44" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="12.9" customHeight="1">
       <c r="A44" s="9">
         <v>36</v>
       </c>
@@ -1633,7 +1724,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="12.9" customHeight="1">
       <c r="A45" s="9">
         <v>37</v>
       </c>
@@ -1657,7 +1748,7 @@
       </c>
       <c r="H45" s="4"/>
     </row>
-    <row r="46" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="12.9" customHeight="1">
       <c r="A46" s="9">
         <v>38</v>
       </c>
@@ -1683,7 +1774,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="12.9" customHeight="1">
       <c r="A47" s="9">
         <v>39</v>
       </c>
@@ -1707,7 +1798,7 @@
       </c>
       <c r="H47" s="4"/>
     </row>
-    <row r="48" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="12.9" customHeight="1">
       <c r="A48" s="9">
         <v>40</v>
       </c>
@@ -1738,8 +1829,8 @@
     <mergeCell ref="A4:H5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" paperSize="1" r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>